<commit_message>
JVM, MongoDB, Angular JS, Jackson
</commit_message>
<xml_diff>
--- a/Definitions/8_Definitions_Angular_JS.xlsx
+++ b/Definitions/8_Definitions_Angular_JS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="148">
   <si>
     <t>Topics</t>
   </si>
@@ -760,6 +760,15 @@
   </si>
   <si>
     <t>AngularJS: Get Started</t>
+  </si>
+  <si>
+    <t>AngularJS: The Big Picture</t>
+  </si>
+  <si>
+    <t>Angular JS Benefits</t>
+  </si>
+  <si>
+    <t>Code Reduction</t>
   </si>
 </sst>
 </file>
@@ -1385,11 +1394,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27:A28"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1786,8 +1795,25 @@
         <v>5</v>
       </c>
     </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B54" s="13"/>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="A54:B54"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A2:B2"/>

</xml_diff>

<commit_message>
Angular JS Definitions - Angular JS: The Big Picture
</commit_message>
<xml_diff>
--- a/Definitions/8_Definitions_Angular_JS.xlsx
+++ b/Definitions/8_Definitions_Angular_JS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="184">
   <si>
     <t>Topics</t>
   </si>
@@ -756,19 +756,157 @@
     <t>Materials</t>
   </si>
   <si>
-    <t>Pluralsight video name</t>
-  </si>
-  <si>
     <t>AngularJS: Get Started</t>
   </si>
   <si>
-    <t>AngularJS: The Big Picture</t>
-  </si>
-  <si>
     <t>Angular JS Benefits</t>
   </si>
   <si>
-    <t>Code Reduction</t>
+    <t>Angular JS Testing tools</t>
+  </si>
+  <si>
+    <t>Karma
+Protractor</t>
+  </si>
+  <si>
+    <t>Cretor of Angular</t>
+  </si>
+  <si>
+    <t>Misko Hevery</t>
+  </si>
+  <si>
+    <t>1. Code Reduction
+2. Two way binding
+3. Cohisive Solution: provides all pieces for web application development
+4. Accessability: using ngAria is making angular more accessible
+5. Internationalization: We can make numbers, dates, currency internationalized. 
+Ex: {{amount | currency}}, {{theDate | date: 'longDate' }}, {{count | number }}
+6. Popularity
+7. Testability: mocking using ngMock. End to End testing with Protractor. Other tools are Karma</t>
+  </si>
+  <si>
+    <t>Basic html attributes to use angular</t>
+  </si>
+  <si>
+    <t>1. ng-app="angular-module-name"
+2. ng-controller="controller-name"</t>
+  </si>
+  <si>
+    <t>handle click event of a button</t>
+  </si>
+  <si>
+    <t>&lt;button ng-click="functionNameInController()" …. /&gt;</t>
+  </si>
+  <si>
+    <t>Pluralsight</t>
+  </si>
+  <si>
+    <t>Angular Js Change detection algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change detection is a process where your framework can tell that some part of the data model has changed and now it needs to update an user interface. Angular uses the concept called dirty checking. The way this works is that angular with little bit of help from developers, simply  watches every event that could change the data. When any of these events happened, angular kicks off digest cycle. This cycle looks to see if any of the data that is being rendered on the page has changed. Angular knows because whenever angular is rendering anything angular makes a copy of that data. Then when data changes angular compares old value with the new value. If any value is changes that means dirty data then angular will re-render that data. </t>
+  </si>
+  <si>
+    <t>Angular Dependency Injection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">function getDate($http){ …. }
+We are using angular to inject http component to our method. In angular components like this are called services. Since it is built-in service it started with $ sign. </t>
+  </si>
+  <si>
+    <t>function calculateCost(items, shippingCalculator) { …. }
+in this case, items and shippingCalculator are services we created. We create these services and register them with angular. So whenever we need these services we simply need to declare them as arguments of method. Angular will inject them</t>
+  </si>
+  <si>
+    <t>Pluralsight - AngularJS: The Big Picture</t>
+  </si>
+  <si>
+    <t>Angular Vs Jquery</t>
+  </si>
+  <si>
+    <t>Angular and Jquery are tied very closely together. Angualar already included min version of Jquery in it's core library. In angular, jquery is used when creating directives (like ng-app etc)</t>
+  </si>
+  <si>
+    <t>Angualr Vs Ionic</t>
+  </si>
+  <si>
+    <t>Ionic is a very interesting framework. It alows us to turn angular application to native phone applications. Ionic is built on top of tool called PhoneGap, which allows a web application to access the native features on a mobile device. Coupled with the ability to compile web app into native phone app. This technique is called hybrid app, since it is a hybrid of both web and native. Developers with angular expertise can learn Ionic with very less efforts</t>
+  </si>
+  <si>
+    <t>Karma and Protractor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tools by angular team to help testing angular applications. </t>
+  </si>
+  <si>
+    <t>Karma: is built on node.  Karma is used to test javascript code. It is not to test html element or page display. It is for testing business logic written in javascript. Karma will watch our files on the disk and when they changed it will re run the tests automatically. Karma will run the code in multiple browsers so that we can make sure code is running as expected in browsers we support. Karma is framework neutral, means it does not care whether code is written in angular, react, or plain venila javascript, It will still run the tests and gives the results.
+Karma is very fast. in most cases it will run the test cases in milli seconds. 
+It is command line tool, so it is to integrate with continuous integration process or any automated process.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protractor: unlike Karma is not meant for just running javascript, it is meant to run code directly in the web page. This is called end-to-end testing. Built on top of another tool called WebDriver.
+WebDriver is a tool that was built to control existing web pages like clicking buttons, writing text to text boxes etc. WebDriver is difficult to use. Protractor over came this difficulty of using WebDrived by adding friendly interface on top of WebDriver. </t>
+  </si>
+  <si>
+    <t>Angular cons and problems</t>
+  </si>
+  <si>
+    <t>1. Browser Compatibility
+2. External Events and How they interact with Digest Cycle: For external events, we need to write custom directives and call angular digest cycle.
+3. SEO
+4. Performance
+5. Very large code bases</t>
+  </si>
+  <si>
+    <t>What's New in Angular 1.3 [Course]</t>
+  </si>
+  <si>
+    <t>Lazy Loading libraries can be used with angular (&lt;= 1.4)
+angular 1.5 has in built lazy loading</t>
+  </si>
+  <si>
+    <t>1. ocLazyLoad
+2. Overmind</t>
+  </si>
+  <si>
+    <t>Angular Vs Old Mvc Frameworks</t>
+  </si>
+  <si>
+    <t>1. Advantage: If we have application already written then better to keep the same. 
+2. Dis Advantage: 
+ 2.1. Buidling application with angular is cheap when compared to using others frameworks
+ 2.2. angular has more features than other frameworks</t>
+  </si>
+  <si>
+    <t>Angular Vs React Advantages</t>
+  </si>
+  <si>
+    <t>1. React is exciting new technology built by a team at Facebook
+2. React is very faster than angular
+3. Has great browser support. Current version of React supports very old versions of IE. So if we want to support IE, we have to consider React.</t>
+  </si>
+  <si>
+    <t>Angular Vs React Dis-Advantages</t>
+  </si>
+  <si>
+    <t>1. Less popular than angular
+2. Suffors from Frankenstein Framework syndrome. Means React by itself is only a rendering engine. It doesn't do other thinks like routing or server communication or any other things angular can do. So we need to use third party tools to build complete application.</t>
+  </si>
+  <si>
+    <t>Angular 2</t>
+  </si>
+  <si>
+    <t>Angular 2 is exciting new feature for the angular framework. In angular 2, team completely revamped the framework to move it forward in a way that really wouldn't be possible without major changes. Angular 2 doesn't have backward compatibility with angular 1. So Angular 2 is like a completely new framework.</t>
+  </si>
+  <si>
+    <t>Why complete change of architecture in Angular 2</t>
+  </si>
+  <si>
+    <t>1. Angular 2 is completely designed with performance in mind
+2. Angular 2 is 5 to 10 times faster than Angular 1
+3. Angular 2 has simplified conceptual model. Angular 2 has removed the idea of controllers and modules. Simplified how service works. Removed configuration overhead. This means learning Angular 2 will be quite straight forward than Angular 1.
+4. Angular 2 is mobile friendly so that both mobile apps and hybrid apps can take the advantage of mobile devices through lower memory and battery needs.
+5. Angular 2 designed keeping web standards in mind. It works well with ECMAScript 6, newest version of javascript and emerging standards like Web Component and Shadow DOM.</t>
   </si>
 </sst>
 </file>
@@ -934,7 +1072,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -967,6 +1105,9 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -984,6 +1125,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1345,17 +1492,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="53.42578125" customWidth="1"/>
-    <col min="2" max="2" width="108.85546875" customWidth="1"/>
+    <col min="1" max="1" width="115.5703125" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1367,17 +1514,22 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="13"/>
+      <c r="B2" s="14"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>143</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1387,24 +1539,26 @@
   <hyperlinks>
     <hyperlink ref="B1" location="Materials!A2" display="Up"/>
     <hyperlink ref="A1" location="Topics!A6" display="Topics"/>
+    <hyperlink ref="A4" r:id="rId1" display="https://app.pluralsight.com/library/courses/angular-1-3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B56"/>
+  <dimension ref="A1:B74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="49.140625" customWidth="1"/>
-    <col min="2" max="2" width="114.42578125" customWidth="1"/>
+    <col min="1" max="1" width="60.140625" customWidth="1"/>
+    <col min="2" max="2" width="125.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1416,10 +1570,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="13"/>
+      <c r="B2" s="14"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
@@ -1446,7 +1600,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="30">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="16" t="s">
         <v>83</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1454,13 +1608,13 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="30">
-      <c r="A7" s="15"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="5" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
         <v>80</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1468,37 +1622,37 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="14"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="14"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="14"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="14"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="14"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="5" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="14"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="5" t="s">
         <v>73</v>
       </c>
@@ -1600,7 +1754,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="60">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="16" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -1608,13 +1762,13 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="60">
-      <c r="A28" s="15"/>
+      <c r="A28" s="16"/>
       <c r="B28" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="16" t="s">
         <v>47</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1622,7 +1776,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="60">
-      <c r="A30" s="15"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="5" t="s">
         <v>45</v>
       </c>
@@ -1636,7 +1790,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="60">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B32" s="5" t="s">
@@ -1644,13 +1798,13 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="60">
-      <c r="A33" s="17"/>
+      <c r="A33" s="18"/>
       <c r="B33" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="120">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1658,13 +1812,13 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="105">
-      <c r="A35" s="15"/>
+      <c r="A35" s="16"/>
       <c r="B35" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="60">
-      <c r="A36" s="15"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="5" t="s">
         <v>36</v>
       </c>
@@ -1718,7 +1872,7 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B43" s="5" t="s">
@@ -1726,7 +1880,7 @@
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="14"/>
+      <c r="A44" s="15"/>
       <c r="B44" s="5" t="s">
         <v>21</v>
       </c>
@@ -1796,23 +1950,169 @@
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="B54" s="13"/>
+      <c r="A54" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B54" s="14"/>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="120">
+      <c r="A56" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="30">
+      <c r="A57" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B57" s="12" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="7" t="s">
-        <v>147</v>
+    <row r="58" spans="1:2" ht="30">
+      <c r="A58" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="90">
+      <c r="A60" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="45">
+      <c r="A61" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="45">
+      <c r="A62" s="19"/>
+      <c r="B62" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="30">
+      <c r="A63" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="60">
+      <c r="A64" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="B65" s="12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="105">
+      <c r="A66" s="20"/>
+      <c r="B66" s="12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="60">
+      <c r="A67" s="20"/>
+      <c r="B67" s="12" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="90">
+      <c r="A68" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="30">
+      <c r="A69" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="B69" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="60">
+      <c r="A70" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="60">
+      <c r="A71" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="B71" s="12" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="45">
+      <c r="A72" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B72" s="12" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="45">
+      <c r="A73" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="B73" s="12" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="120">
+      <c r="A74" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B74" s="12" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A65:A67"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="A34:A36"/>
@@ -1858,10 +2158,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13"/>
+      <c r="B2" s="14"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
@@ -2046,7 +2346,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2064,10 +2364,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="13"/>
+      <c r="B2" s="14"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="9" t="s">
@@ -2167,7 +2467,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>

<commit_message>
Angular Js + Github
</commit_message>
<xml_diff>
--- a/Definitions/8_Definitions_Angular_JS.xlsx
+++ b/Definitions/8_Definitions_Angular_JS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="194">
   <si>
     <t>Topics</t>
   </si>
@@ -907,6 +907,36 @@
 3. Angular 2 has simplified conceptual model. Angular 2 has removed the idea of controllers and modules. Simplified how service works. Removed configuration overhead. This means learning Angular 2 will be quite straight forward than Angular 1.
 4. Angular 2 is mobile friendly so that both mobile apps and hybrid apps can take the advantage of mobile devices through lower memory and battery needs.
 5. Angular 2 designed keeping web standards in mind. It works well with ECMAScript 6, newest version of javascript and emerging standards like Web Component and Shadow DOM.</t>
+  </si>
+  <si>
+    <t>Pluralsight - AngularJS: Get Started</t>
+  </si>
+  <si>
+    <t>Different applications/products built with angular js</t>
+  </si>
+  <si>
+    <t>https://www.madewithangular.com/</t>
+  </si>
+  <si>
+    <t>Angular JS online IDE</t>
+  </si>
+  <si>
+    <t>http://plnkr.co/</t>
+  </si>
+  <si>
+    <t>Click "Launch the Editor" button</t>
+  </si>
+  <si>
+    <t>Application Directive</t>
+  </si>
+  <si>
+    <t>F12</t>
+  </si>
+  <si>
+    <t>Chrome Developer Tools short cut key</t>
+  </si>
+  <si>
+    <t>Immediately Invoked Function Expression (IIFE) to avoid global variables</t>
   </si>
 </sst>
 </file>
@@ -1072,7 +1102,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1108,11 +1138,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1126,11 +1168,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1514,10 +1553,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="14"/>
+      <c r="B2" s="16"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
@@ -1548,11 +1587,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B74"/>
+  <dimension ref="A1:B82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1570,10 +1609,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="14"/>
+      <c r="B2" s="16"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
@@ -1600,7 +1639,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="30">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="20" t="s">
         <v>83</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1608,13 +1647,13 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="30">
-      <c r="A7" s="16"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="5" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="21" t="s">
         <v>80</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1622,37 +1661,37 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="15"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="15"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="15"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="15"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="15"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="5" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="15"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="5" t="s">
         <v>73</v>
       </c>
@@ -1681,7 +1720,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="30">
+    <row r="18" spans="1:2">
       <c r="A18" s="5" t="s">
         <v>67</v>
       </c>
@@ -1754,7 +1793,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="60">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="20" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -1762,13 +1801,13 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="60">
-      <c r="A28" s="16"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="20" t="s">
         <v>47</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1776,7 +1815,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="60">
-      <c r="A30" s="16"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="5" t="s">
         <v>45</v>
       </c>
@@ -1790,7 +1829,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="60">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="22" t="s">
         <v>42</v>
       </c>
       <c r="B32" s="5" t="s">
@@ -1798,13 +1837,13 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="60">
-      <c r="A33" s="18"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="120">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="20" t="s">
         <v>39</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1812,18 +1851,18 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="105">
-      <c r="A35" s="16"/>
+      <c r="A35" s="20"/>
       <c r="B35" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="60">
-      <c r="A36" s="16"/>
+      <c r="A36" s="20"/>
       <c r="B36" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="105">
+    <row r="37" spans="1:2" ht="90">
       <c r="A37" s="5" t="s">
         <v>35</v>
       </c>
@@ -1872,7 +1911,7 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="15" t="s">
+      <c r="A43" s="19" t="s">
         <v>23</v>
       </c>
       <c r="B43" s="5" t="s">
@@ -1880,7 +1919,7 @@
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="15"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="5" t="s">
         <v>21</v>
       </c>
@@ -1925,7 +1964,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="60">
+    <row r="50" spans="1:2" ht="45">
       <c r="A50" s="5" t="s">
         <v>10</v>
       </c>
@@ -1950,10 +1989,10 @@
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="13" t="s">
+      <c r="A54" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="B54" s="14"/>
+      <c r="B54" s="16"/>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="7" t="s">
@@ -2004,7 +2043,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" ht="45">
-      <c r="A61" s="19" t="s">
+      <c r="A61" s="17" t="s">
         <v>157</v>
       </c>
       <c r="B61" s="12" t="s">
@@ -2012,7 +2051,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" ht="45">
-      <c r="A62" s="19"/>
+      <c r="A62" s="17"/>
       <c r="B62" s="12" t="s">
         <v>159</v>
       </c>
@@ -2034,7 +2073,7 @@
       </c>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" s="20" t="s">
+      <c r="A65" s="18" t="s">
         <v>165</v>
       </c>
       <c r="B65" s="12" t="s">
@@ -2042,13 +2081,13 @@
       </c>
     </row>
     <row r="66" spans="1:2" ht="105">
-      <c r="A66" s="20"/>
+      <c r="A66" s="18"/>
       <c r="B66" s="12" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="60">
-      <c r="A67" s="20"/>
+      <c r="A67" s="18"/>
       <c r="B67" s="12" t="s">
         <v>168</v>
       </c>
@@ -2109,19 +2148,73 @@
         <v>183</v>
       </c>
     </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="B76" s="16"/>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="B77" s="23" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="18"/>
+      <c r="B79" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>91</v>
+      </c>
+      <c r="B80" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>192</v>
+      </c>
+      <c r="B81" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="150">
+      <c r="A82" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A27:A28"/>
     <mergeCell ref="A61:A62"/>
     <mergeCell ref="A65:A67"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A32:A33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Topics!A2" display="Topics"/>
@@ -2129,6 +2222,8 @@
     <hyperlink ref="B23" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B77" r:id="rId4"/>
+    <hyperlink ref="B78" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2158,10 +2253,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="14"/>
+      <c r="B2" s="16"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
@@ -2364,10 +2459,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="14"/>
+      <c r="B2" s="16"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="9" t="s">

</xml_diff>

<commit_message>
OAuth 2, JWT, Open ID Connect
</commit_message>
<xml_diff>
--- a/Definitions/8_Definitions_Angular_JS.xlsx
+++ b/Definitions/8_Definitions_Angular_JS.xlsx
@@ -8,17 +8,18 @@
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="1" r:id="rId1"/>
-    <sheet name="Definitions" sheetId="2" r:id="rId2"/>
+    <sheet name="Angular 1" sheetId="2" r:id="rId2"/>
     <sheet name="Directives" sheetId="3" r:id="rId3"/>
     <sheet name="Services" sheetId="4" r:id="rId4"/>
     <sheet name="Routing" sheetId="5" r:id="rId5"/>
+    <sheet name="Angular 2" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="222">
   <si>
     <t>Topics</t>
   </si>
@@ -132,13 +133,6 @@
     <t>Filters basic format</t>
   </si>
   <si>
-    <t>* Controllers usually live in modules - this avoids global namespace
-* Working with modules - Create a module with a name. (Ex: var app = angular.module("githubviewer", []); 
-angular is only global object to use anywhere in angular project. githubviewer == name of the module. [] == array of dependencies of this modules. if empty array then no explicit dependencies but implicitly it depends on core angular modules
-* Register controller to module (Ex: app.controller("MainController", MainController);
-* Tell angular to use your module with ng-app (Ex: &lt;body ng-app="githubviewer"&gt; ... &lt;/body&gt;</t>
-  </si>
-  <si>
     <t>Modules</t>
   </si>
   <si>
@@ -168,53 +162,6 @@
   </si>
   <si>
     <t>How to make server calls in Angular JS</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">&lt;img </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ng-src</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">="{{person.imageSrc}}" title="{{person.firstName}} {{peson.lastName}}" height="200px;" width="200px;"/&gt;
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> if we use like following, we will get 404-not found error in broser console because browser finds img tag src, it will try to download the image after that browser binds angula controller. &lt;img src="{{person.imageSrc}}" title="{{person.firstName}} {{peson.lastName}}" height="200px;" width="200px;"/&gt;</t>
-    </r>
   </si>
   <si>
     <r>
@@ -293,12 +240,6 @@
 Ex: var MyController = function($scope){ 
 $scope.message = "Hello"; 
 };</t>
-  </si>
-  <si>
-    <t>Controller directive in html (ng-controller). Ng-controller is an attribute. 
-Ex: &lt;div ng-app&gt;   --&gt; ng-app will Initialize Angular
-&lt;div ng-controller="MyController"&gt; …. &lt;/div&gt;
-&lt;/div&gt;</t>
   </si>
   <si>
     <t>Controller Basics</t>
@@ -501,14 +442,6 @@
     </r>
   </si>
   <si>
-    <t>1. Directives
-2. Data Binding
-3. Filters
-4. Modules
-5. Routes
-6. Controllers</t>
-  </si>
-  <si>
     <t>Core features of Angular JS</t>
   </si>
   <si>
@@ -745,13 +678,6 @@
     <t>We need to give routing rules using $routeProvider</t>
   </si>
   <si>
-    <t>$routeProvider
-     .when("/main", {
-                    templateUrl: "main.html",
-                    controller: "MainController"
-});</t>
-  </si>
-  <si>
     <t>Materials</t>
   </si>
   <si>
@@ -763,9 +689,6 @@
   <si>
     <t>Karma
 Protractor</t>
-  </si>
-  <si>
-    <t>Cretor of Angular</t>
   </si>
   <si>
     <t>Misko Hevery</t>
@@ -800,9 +723,6 @@
     <t>Angular Js Change detection algorithm</t>
   </si>
   <si>
-    <t xml:space="preserve">Change detection is a process where your framework can tell that some part of the data model has changed and now it needs to update an user interface. Angular uses the concept called dirty checking. The way this works is that angular with little bit of help from developers, simply  watches every event that could change the data. When any of these events happened, angular kicks off digest cycle. This cycle looks to see if any of the data that is being rendered on the page has changed. Angular knows because whenever angular is rendering anything angular makes a copy of that data. Then when data changes angular compares old value with the new value. If any value is changes that means dirty data then angular will re-render that data. </t>
-  </si>
-  <si>
     <t>Angular Dependency Injection</t>
   </si>
   <si>
@@ -838,10 +758,6 @@
     <t>Karma: is built on node.  Karma is used to test javascript code. It is not to test html element or page display. It is for testing business logic written in javascript. Karma will watch our files on the disk and when they changed it will re run the tests automatically. Karma will run the code in multiple browsers so that we can make sure code is running as expected in browsers we support. Karma is framework neutral, means it does not care whether code is written in angular, react, or plain venila javascript, It will still run the tests and gives the results.
 Karma is very fast. in most cases it will run the test cases in milli seconds. 
 It is command line tool, so it is to integrate with continuous integration process or any automated process.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protractor: unlike Karma is not meant for just running javascript, it is meant to run code directly in the web page. This is called end-to-end testing. Built on top of another tool called WebDriver.
-WebDriver is a tool that was built to control existing web pages like clicking buttons, writing text to text boxes etc. WebDriver is difficult to use. Protractor over came this difficulty of using WebDrived by adding friendly interface on top of WebDriver. </t>
   </si>
   <si>
     <t>Angular cons and problems</t>
@@ -885,10 +801,6 @@
     <t>Angular Vs React Dis-Advantages</t>
   </si>
   <si>
-    <t>1. Less popular than angular
-2. Suffors from Frankenstein Framework syndrome. Means React by itself is only a rendering engine. It doesn't do other thinks like routing or server communication or any other things angular can do. So we need to use third party tools to build complete application.</t>
-  </si>
-  <si>
     <t>Angular 2</t>
   </si>
   <si>
@@ -968,6 +880,147 @@
   </si>
   <si>
     <t>AngularJS: Get Started [Course]</t>
+  </si>
+  <si>
+    <t>Angular: First Look</t>
+  </si>
+  <si>
+    <t>Angular Fundamentals</t>
+  </si>
+  <si>
+    <t>Angular: Getting Started [Course]</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=-zW1zHqsdyc</t>
+  </si>
+  <si>
+    <t>Youtube - Angular 2 in 60 minutes</t>
+  </si>
+  <si>
+    <t>An AngularJS Playbook</t>
+  </si>
+  <si>
+    <t>Building Components with Angular 1.5</t>
+  </si>
+  <si>
+    <t>AngularJS Security Fundamentals [Course]</t>
+  </si>
+  <si>
+    <t>AngularJS Application Development [Course]</t>
+  </si>
+  <si>
+    <t>AngularJS Best Practices [Course]</t>
+  </si>
+  <si>
+    <t>AngularJS Directives Fundamentals [Course]</t>
+  </si>
+  <si>
+    <t>AngularJS Forms Using Bootstrap and MVC 5 [Course]</t>
+  </si>
+  <si>
+    <t>AngularJS Front to Back with Web API [Course]</t>
+  </si>
+  <si>
+    <t>AngularJS In-Depth [Course]</t>
+  </si>
+  <si>
+    <t>AngularJS Patterns: Clean Code [Course]</t>
+  </si>
+  <si>
+    <t>AngularJS Routing In-depth [Course]</t>
+  </si>
+  <si>
+    <t>AngularJS Services In-depth [Course]</t>
+  </si>
+  <si>
+    <t>AngularJS Unit Testing in-depth, Using ngMock [Course]</t>
+  </si>
+  <si>
+    <t>1. Modules
+2. Controllers
+3. Directives
+4. Data Binding
+5. Filters
+6. Routes</t>
+  </si>
+  <si>
+    <t>Controller directive in html (ng-controller). ng-controller is an attribute. 
+Ex: &lt;div ng-app&gt;   --&gt; ng-app will Initialize Angular
+&lt;div ng-controller="MyController"&gt; …. &lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;img </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ng-src</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">="{{person.imageSrc}}" title="{{person.firstName}} {{peson.lastName}}" height="200px;" width="200px;"/&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> if we use like following, we will get 404-not found error in browser console because whenever browser finds img tag src, it will try to download the image after that browser binds angula controller. 
+&lt;img src="{{person.imageSrc}}" title="{{person.firstName}} {{peson.lastName}}" height="200px;" width="200px;"/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Controllers usually live in modules - this avoids global namespace
+2. Working with modules - Create a module with a name. (Ex: var app = angular.module("githubviewer", []); 
+angular is only global object to use anywhere in angular project. githubviewer == name of the module. [] == array of dependencies of this modules. if empty array then no explicit dependencies but implicitly it depends on core angular modules
+3. Register controller to module (Ex: app.controller("MainController", MainController);
+4. Tell angular to use your module with ng-app (Ex: &lt;body ng-app="githubviewer"&gt; ... &lt;/body&gt;</t>
+  </si>
+  <si>
+    <t>Creator of Angular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change detection is a process where your framework can tell that some part of the data model has changed and now it needs to update an user interface. Angular uses the concept called dirty checking. The way this works is that angular with little bit of help from developers, simply  watches every event that could change the data. When any of these events happened, angular kicks off digest cycle. This cycle looks to see if any of the data that is being rendered on the page has changed. Angular knows because whenever angular is rendering anything angular makes a copy of that data. Then when data changes angular compares old value with the new value. If any value is changed that means dirty data then angular will re-render that data. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protractor: unlike Karma is not meant for just running javascript, it is meant to run code directly in the web page. This is called end-to-end testing. Built on top of another tool called WebDriver.
+WebDriver is a tool that was built to control existing web pages like clicking buttons, writing text to text boxes etc. WebDriver is difficult to use. Protractor over came this difficulty of using WebDriver by adding friendly interface on top of WebDriver. </t>
+  </si>
+  <si>
+    <t>1. Less popular than angular
+2. Suffors from Frankenstein Framework syndrome. Means React by itself is only a rendering engine. It doesn't do other things like routing or server communication or any other things angular can do. So we need to use third party tools to build complete application.</t>
+  </si>
+  <si>
+    <t>$routeProvider
+ .when( "/main", { templateUrl: "main.html", controller: "MainController" } );</t>
   </si>
 </sst>
 </file>
@@ -1038,7 +1091,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1072,12 +1125,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF33CC33"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1139,7 +1186,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1193,8 +1240,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1225,6 +1276,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1523,7 +1580,8 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1557,19 +1615,22 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>170</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A4" location="Services!A1" display="Services"/>
     <hyperlink ref="A3" location="Directives!A1" display="Directives"/>
-    <hyperlink ref="A2" location="Definitions!A1" display="Definitions"/>
+    <hyperlink ref="A2" location="'Angular 1'!A1" display="Definitions"/>
     <hyperlink ref="B1" location="Topics!A2" display="Up"/>
     <hyperlink ref="A5" location="Routing!A1" display="Routing"/>
+    <hyperlink ref="A6" location="'Angular 2'!A1" display="Angular 2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1577,11 +1638,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B99"/>
+  <dimension ref="A1:B112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1600,729 +1661,846 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="21" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B2" s="22"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="18" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
+      <c r="A5" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
+      <c r="A6" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B6" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="31" t="s">
         <v>201</v>
       </c>
-      <c r="B7" s="24"/>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="B16" s="22"/>
+      <c r="B16" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>88</v>
+      <c r="A17" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="B17" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B18" s="8" t="s">
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="B20" s="24"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="21" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="5" t="s">
+      <c r="B29" s="22"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B30" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="30">
-      <c r="A20" s="29" t="s">
+    <row r="31" spans="1:2">
+      <c r="A31" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B31" s="8" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="30">
-      <c r="A21" s="29"/>
-      <c r="B21" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="28"/>
-      <c r="B23" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="28"/>
-      <c r="B24" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="28"/>
-      <c r="B25" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="28"/>
-      <c r="B26" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="28"/>
-      <c r="B27" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="28"/>
-      <c r="B28" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="90">
-      <c r="A29" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="75">
-      <c r="A30" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="75">
-      <c r="A31" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="30">
+      <c r="A33" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="30">
+      <c r="A34" s="29"/>
+      <c r="B34" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="28"/>
+      <c r="B36" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="28"/>
+      <c r="B37" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="28"/>
+      <c r="B38" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="28"/>
+      <c r="B39" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="28"/>
+      <c r="B40" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="28"/>
+      <c r="B41" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="90">
+      <c r="A42" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="75">
+      <c r="A43" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="5" t="s">
+    </row>
+    <row r="44" spans="1:2" ht="75">
+      <c r="A44" s="5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="30">
-      <c r="A33" s="5" t="s">
+      <c r="B44" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="30">
+      <c r="A46" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="30">
+      <c r="A47" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="45">
+      <c r="A48" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="30">
+      <c r="A49" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="45">
+      <c r="A52" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="150">
+      <c r="A53" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="60">
+      <c r="A54" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="60">
+      <c r="A55" s="29"/>
+      <c r="B55" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="60">
+      <c r="A57" s="29"/>
+      <c r="B57" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="60">
+      <c r="A58" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="60">
+      <c r="A59" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="60">
+      <c r="A60" s="25"/>
+      <c r="B60" s="19" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="120">
+      <c r="A61" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="105">
+      <c r="A62" s="29"/>
+      <c r="B62" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="60">
+      <c r="A63" s="29"/>
+      <c r="B63" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="30">
-      <c r="A34" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="45">
-      <c r="A35" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="30">
-      <c r="A36" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="45">
-      <c r="A39" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="150">
-      <c r="A40" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="60">
-      <c r="A41" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="60">
-      <c r="A42" s="29"/>
-      <c r="B42" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="60">
-      <c r="A44" s="29"/>
-      <c r="B44" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="60">
-      <c r="A45" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="60">
-      <c r="A46" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="60">
-      <c r="A47" s="25"/>
-      <c r="B47" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="120">
-      <c r="A48" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="105">
-      <c r="A49" s="29"/>
-      <c r="B49" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="60">
-      <c r="A50" s="29"/>
-      <c r="B50" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="90">
-      <c r="A51" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B51" s="5" t="s">
+    </row>
+    <row r="64" spans="1:2" ht="90">
+      <c r="A64" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" ht="30">
-      <c r="A52" s="5" t="s">
+      <c r="B64" s="19" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="30">
+      <c r="A65" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B65" s="5" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="28"/>
-      <c r="B58" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="45">
-      <c r="A64" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="135">
-      <c r="A65" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="28"/>
+      <c r="B71" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="45">
+      <c r="A77" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="135">
+      <c r="A78" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B79" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="B68" s="22"/>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="7" t="s">
+    <row r="81" spans="1:2">
+      <c r="A81" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="B81" s="22"/>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="120">
+      <c r="A83" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B83" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="30">
+      <c r="A84" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B84" s="11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="30">
+      <c r="A85" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B85" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B86" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="B69" s="7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="120">
-      <c r="A70" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="B70" s="11" t="s">
+    </row>
+    <row r="87" spans="1:2" ht="90">
+      <c r="A87" s="7" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" ht="30">
-      <c r="A71" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="B71" s="11" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="30">
-      <c r="A72" s="7" t="s">
+      <c r="B87" s="19" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="45">
+      <c r="A88" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="B72" s="11" t="s">
+      <c r="B88" s="11" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="7" t="s">
+    <row r="89" spans="1:2" ht="45">
+      <c r="A89" s="30"/>
+      <c r="B89" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="B73" s="11" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="90">
-      <c r="A74" s="7" t="s">
+    </row>
+    <row r="90" spans="1:2" ht="30">
+      <c r="A90" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B90" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="B74" s="11" t="s">
+    </row>
+    <row r="91" spans="1:2" ht="60">
+      <c r="A91" s="7" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" ht="45">
-      <c r="A75" s="30" t="s">
+      <c r="B91" s="11" t="s">
         <v>156</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="45">
-      <c r="A76" s="30"/>
-      <c r="B76" s="11" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="30">
-      <c r="A77" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="B77" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="60">
-      <c r="A78" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="B78" s="11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="B79" s="11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="105">
-      <c r="A80" s="26"/>
-      <c r="B80" s="11" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="60">
-      <c r="A81" s="26"/>
-      <c r="B81" s="11" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="90">
-      <c r="A82" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="B82" s="11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="30">
-      <c r="A83" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="B83" s="11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="60">
-      <c r="A84" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="B84" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="60">
-      <c r="A85" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="B85" s="11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="45">
-      <c r="A86" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="B86" s="11" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="45">
-      <c r="A87" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="B87" s="11" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="120">
-      <c r="A88" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="B88" s="11" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="21" t="s">
-        <v>183</v>
-      </c>
-      <c r="B90" s="22"/>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="B91" s="15" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="B92" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="105">
+      <c r="A93" s="26"/>
+      <c r="B93" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="60">
+      <c r="A94" s="26"/>
+      <c r="B94" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="90">
+      <c r="A95" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B95" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="30">
+      <c r="A96" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B96" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="60">
+      <c r="A97" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B97" s="11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="60">
+      <c r="A98" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B98" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="45">
+      <c r="A99" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="B99" s="19" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="45">
+      <c r="A100" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B100" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="120">
+      <c r="A101" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B101" s="11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="B103" s="22"/>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="B104" s="15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="26"/>
+      <c r="B106" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>87</v>
+      </c>
+      <c r="B107" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>182</v>
+      </c>
+      <c r="B108" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="150">
+      <c r="A109" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B109" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="30">
+      <c r="A110" t="s">
+        <v>184</v>
+      </c>
+      <c r="B110" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="B92" s="1" t="s">
+    </row>
+    <row r="111" spans="1:2" ht="30">
+      <c r="A111" t="s">
+        <v>185</v>
+      </c>
+      <c r="B111" s="14" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="26"/>
-      <c r="B93" t="s">
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" t="s">
-        <v>91</v>
-      </c>
-      <c r="B94" t="s">
+      <c r="B112" s="14" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" t="s">
-        <v>191</v>
-      </c>
-      <c r="B95" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="150">
-      <c r="A96" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="B96" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="30">
-      <c r="A97" t="s">
-        <v>193</v>
-      </c>
-      <c r="B97" s="14" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="30">
-      <c r="A98" t="s">
-        <v>194</v>
-      </c>
-      <c r="B98" s="14" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="A99" t="s">
-        <v>197</v>
-      </c>
-      <c r="B99" s="14" t="s">
-        <v>198</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A105:A106"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A35:A41"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="A92:A94"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="A61:A63"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Topics!A2" display="Topics"/>
     <hyperlink ref="B1" location="Definitions!A2" display="Up"/>
-    <hyperlink ref="B37" r:id="rId1"/>
-    <hyperlink ref="B17" r:id="rId2"/>
-    <hyperlink ref="B18" r:id="rId3"/>
-    <hyperlink ref="B91" r:id="rId4"/>
-    <hyperlink ref="B92" r:id="rId5"/>
+    <hyperlink ref="B50" r:id="rId1"/>
+    <hyperlink ref="B30" r:id="rId2"/>
+    <hyperlink ref="B31" r:id="rId3"/>
+    <hyperlink ref="B104" r:id="rId4"/>
+    <hyperlink ref="B105" r:id="rId5"/>
     <hyperlink ref="A3" r:id="rId6"/>
-    <hyperlink ref="A9" r:id="rId7" display="https://app.pluralsight.com/library/courses/angularjs-get-started"/>
-    <hyperlink ref="A8" r:id="rId8" display="https://app.pluralsight.com/library/courses/angular-big-picture"/>
-    <hyperlink ref="A4" r:id="rId9" display="https://app.pluralsight.com/library/courses/angular-1-3"/>
+    <hyperlink ref="A22" r:id="rId7" display="https://app.pluralsight.com/library/courses/angularjs-get-started"/>
+    <hyperlink ref="A4" r:id="rId8" display="https://app.pluralsight.com/library/courses/angular-1-3"/>
+    <hyperlink ref="A21" r:id="rId9" display="https://app.pluralsight.com/library/courses/angular-big-picture"/>
+    <hyperlink ref="A17" r:id="rId10" tooltip="An AngularJS Playbook" display="https://app.pluralsight.com/library/courses/angularjs-playbook"/>
+    <hyperlink ref="A16" r:id="rId11" tooltip="Building Components with Angular 1.5" display="https://app.pluralsight.com/library/courses/building-components-angular-1-5"/>
+    <hyperlink ref="A14" r:id="rId12" display="https://app.pluralsight.com/library/courses/angular-application-development"/>
+    <hyperlink ref="A13" r:id="rId13" display="https://app.pluralsight.com/library/courses/angular-best-practices"/>
+    <hyperlink ref="A12" r:id="rId14" display="https://app.pluralsight.com/library/courses/angularjs-directive-fundamentals"/>
+    <hyperlink ref="A11" r:id="rId15" display="https://app.pluralsight.com/library/courses/angularjs-forms-bootstrap-mvc5"/>
+    <hyperlink ref="A10" r:id="rId16" display="https://app.pluralsight.com/library/courses/angular-web-api-front-back"/>
+    <hyperlink ref="A9" r:id="rId17" display="https://app.pluralsight.com/library/courses/angularjs-in-depth"/>
+    <hyperlink ref="A8" r:id="rId18" display="https://app.pluralsight.com/library/courses/angularjs-patterns-clean-code"/>
+    <hyperlink ref="A7" r:id="rId19" display="https://app.pluralsight.com/library/courses/angular-routing-in-depth"/>
+    <hyperlink ref="A6" r:id="rId20" display="https://app.pluralsight.com/library/courses/angularjs-services-in-depth"/>
+    <hyperlink ref="A5" r:id="rId21" display="https://app.pluralsight.com/library/courses/angularjs-ngmock-unit-testing"/>
+    <hyperlink ref="A15" r:id="rId22" display="https://app.pluralsight.com/library/courses/angularjs-security-fundamentals"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
 
@@ -2357,167 +2535,167 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2563,21 +2741,21 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B4" s="5"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B5" s="5"/>
     </row>
@@ -2595,52 +2773,52 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B9" s="5"/>
     </row>
     <row r="10" spans="1:2" ht="30">
       <c r="A10" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B11" s="5"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B12" s="5"/>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="60">
       <c r="A14" s="5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2659,7 +2837,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2677,18 +2857,18 @@
     </row>
     <row r="2" spans="1:2" ht="30">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="75">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30">
       <c r="A3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>141</v>
+        <v>136</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2699,4 +2879,104 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="80.140625" customWidth="1"/>
+    <col min="2" max="2" width="107" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="22"/>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="B10" s="22"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A15:B15"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B1" location="'Angular 2'!A2" display="Up"/>
+    <hyperlink ref="A1" location="Topics!A6" display="Topics"/>
+    <hyperlink ref="A3" r:id="rId1" tooltip="Angular: First Look" display="https://app.pluralsight.com/library/courses/angular-2-first-look"/>
+    <hyperlink ref="A4" r:id="rId2" tooltip="Angular Fundamentals" display="https://app.pluralsight.com/library/courses/angularjs-fundamentals"/>
+    <hyperlink ref="A5" r:id="rId3" display="https://app.pluralsight.com/library/courses/angular-2-getting-started-update"/>
+    <hyperlink ref="A6" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
SQL, angular Js, ORM
</commit_message>
<xml_diff>
--- a/Definitions/8_Definitions_Angular_JS.xlsx
+++ b/Definitions/8_Definitions_Angular_JS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="1" r:id="rId1"/>
@@ -1646,9 +1646,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2891,7 +2891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>

</xml_diff>